<commit_message>
Almost through SuRGE processing.  Hopefully I haven't broken anything.
</commit_message>
<xml_diff>
--- a/inst/extdata/ext_chla_2021_theirs_spec.xlsx
+++ b/inst/extdata/ext_chla_2021_theirs_spec.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/shivers_stephen_epa_gov/Documents/2021_03_02/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JHollist\projects\compeco\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0697CAF-3777-4CD1-A3E7-8B1157DF1616}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455EF2C5-7692-461C-99D8-E5A1EEF906EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="16200" windowHeight="9360" firstSheet="1" activeTab="1" xr2:uid="{58FD136C-537E-43D8-88F9-37BEC1397E1B}"/>
+    <workbookView xWindow="2340" yWindow="0" windowWidth="23085" windowHeight="15600" activeTab="6" xr2:uid="{58FD136C-537E-43D8-88F9-37BEC1397E1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Blank.Sample" sheetId="1" r:id="rId1"/>
-    <sheet name="E.Sample" sheetId="2" r:id="rId2"/>
-    <sheet name="D.Sample" sheetId="3" r:id="rId3"/>
-    <sheet name="C.Sample" sheetId="4" r:id="rId4"/>
-    <sheet name="B.Sample" sheetId="5" r:id="rId5"/>
-    <sheet name="A.Sample" sheetId="6" r:id="rId6"/>
-    <sheet name="F.Sample" sheetId="7" r:id="rId7"/>
+    <sheet name="F.Sample" sheetId="2" r:id="rId2"/>
+    <sheet name="E.Sample" sheetId="3" r:id="rId3"/>
+    <sheet name="D.Sample" sheetId="4" r:id="rId4"/>
+    <sheet name="C.Sample" sheetId="5" r:id="rId5"/>
+    <sheet name="B.Sample" sheetId="6" r:id="rId6"/>
+    <sheet name="A.Sample" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1670,7 +1670,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8388D6EC-B6B0-43C5-9482-758545E69E01}">
   <dimension ref="A2:B156"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A16" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -6606,7 +6606,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E92826EA-D64E-4CD8-A424-380648288CFC}">
   <dimension ref="A2:B156"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -7840,7 +7842,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67090DAA-8AE8-412F-B4AB-6A53E9843AE8}">
   <dimension ref="A2:B156"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="M75" sqref="M75"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>